<commit_message>
separated water and city administrator comparisons
</commit_message>
<xml_diff>
--- a/maumee-comparison.xlsx
+++ b/maumee-comparison.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Water &amp; Sewer Rates" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="City Administrator Salaries" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t xml:space="preserve">City/Municipality</t>
   </si>
@@ -618,63 +617,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://maumee.org/download/ordinance-015-2024/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 Median Household Income***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Administrator Name (as of 2022)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reported Title (as of 2022)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 Salary*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salary-to-Population Ratio ($ of salary per resident)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lori Trettor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipal Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridgette Kabat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin Aller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Of Public Service Safety Director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dale Thornton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeffery Leonard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenneth Frost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety/Service Director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patrick Burtch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Admin Safety &amp; Serv Dir</t>
   </si>
 </sst>
 </file>
@@ -779,7 +721,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,10 +820,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -893,7 +831,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1037,30 +975,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF17B02F"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF79D11B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
 </styleSheet>
 </file>
@@ -1165,126 +1079,6 @@
             <a:t>4. If you find a mistake please let me know at waterrates@funkybeluga.com</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>30240</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>120600</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="Text Frame 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="30240" y="4823280"/>
-          <a:ext cx="5636520" cy="569160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-            </a:rPr>
-            <a:t>Notes</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-            </a:rPr>
-            <a:t>* According to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-              <a:hlinkClick r:id="rId1"/>
-            </a:rPr>
-            <a:t>https://govsalaries.com/</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-            </a:rPr>
-            <a:t>** The larger cities don’t have a position commensurate with Maumee’s City Administrator position</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-            </a:rPr>
-            <a:t>*** According to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
-              <a:uFillTx/>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Noto Sans CJK SC"/>
-              <a:hlinkClick r:id="rId2"/>
-            </a:rPr>
-            <a:t>https://www.city-data.com/</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1000" strike="noStrike" u="none">
             <a:uFillTx/>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -1410,7 +1204,7 @@
   <dimension ref="A1:XFD11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2040,8 +1834,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="15" t="n">
-        <f aca="false">7.34*1.3368</f>
-        <v>9.812112</v>
+        <v>9.81</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>44</v>
@@ -2055,15 +1848,15 @@
       </c>
       <c r="K8" s="15" t="n">
         <f aca="false">IF($I8&gt;3000,(VALUE($J8)),($J8+((3000-$I8)/1000*($E8+$G8))))</f>
-        <v>124.446336</v>
+        <v>124.44</v>
       </c>
       <c r="L8" s="15" t="n">
         <f aca="false">IF($I8&gt;6000,(VALUE($J8)),($J8+((6000-$I8)/1000*($E8+$G8))))</f>
-        <v>191.892672</v>
+        <v>191.88</v>
       </c>
       <c r="M8" s="15" t="n">
         <f aca="false">IF($I8&gt;12000,(VALUE($J8)),($J8+((12000-$I8)/1000*($E8+$G8))))</f>
-        <v>326.785344</v>
+        <v>326.76</v>
       </c>
       <c r="N8" s="19" t="n">
         <f aca="false">19*3</f>
@@ -2071,15 +1864,15 @@
       </c>
       <c r="O8" s="19" t="n">
         <f aca="false">IF($I8&gt;3000,(VALUE($N8)),($N8+((3000-$I8)/1000*($E8+$G8))))</f>
-        <v>124.446336</v>
+        <v>124.44</v>
       </c>
       <c r="P8" s="19" t="n">
         <f aca="false">IF($I8&gt;6000,(VALUE($N8)),($N8+((6000-$I8)/1000*($E8+$G8))))</f>
-        <v>191.892672</v>
+        <v>191.88</v>
       </c>
       <c r="Q8" s="19" t="n">
         <f aca="false">IF($I8&gt;12000,(VALUE($N8)),($N8+((12000-$I8)/1000*($E8+$G8))))</f>
-        <v>326.785344</v>
+        <v>326.76</v>
       </c>
       <c r="R8" s="19" t="n">
         <f aca="false">81.35/2*3</f>
@@ -2087,15 +1880,15 @@
       </c>
       <c r="S8" s="19" t="n">
         <f aca="false">IF($I8&gt;3000,(VALUE($R8)),($R8+((3000-$I8)/1000*($E8+$G8))))</f>
-        <v>189.471336</v>
+        <v>189.465</v>
       </c>
       <c r="T8" s="19" t="n">
         <f aca="false">IF($I8&gt;6000,(VALUE($R8)),($R8+((6000-$I8)/1000*($E8+$G8))))</f>
-        <v>256.917672</v>
+        <v>256.905</v>
       </c>
       <c r="U8" s="19" t="n">
         <f aca="false">IF($I8&gt;12000,(VALUE($R8)),($R8+((12000-$I8)/1000*($E8+$G8))))</f>
-        <v>391.810344</v>
+        <v>391.785</v>
       </c>
       <c r="V8" s="21" t="s">
         <v>45</v>
@@ -2514,801 +2307,4 @@
   </headerFooter>
   <drawing r:id="rId8"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:XFD11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="9.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16363" min="9" style="6" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="XEJ1" s="0"/>
-      <c r="XEK1" s="0"/>
-      <c r="XEL1" s="0"/>
-      <c r="XEM1" s="0"/>
-      <c r="XEN1" s="0"/>
-      <c r="XEO1" s="0"/>
-      <c r="XEP1" s="0"/>
-      <c r="XEQ1" s="0"/>
-      <c r="XER1" s="0"/>
-      <c r="XES1" s="0"/>
-      <c r="XET1" s="0"/>
-      <c r="XEU1" s="0"/>
-      <c r="XEV1" s="0"/>
-      <c r="XEW1" s="0"/>
-      <c r="XEX1" s="0"/>
-      <c r="XEY1" s="0"/>
-      <c r="XEZ1" s="0"/>
-      <c r="XFA1" s="0"/>
-      <c r="XFB1" s="0"/>
-      <c r="XFC1" s="0"/>
-      <c r="XFD1" s="0"/>
-    </row>
-    <row r="2" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="12" t="n">
-        <v>270871</v>
-      </c>
-      <c r="C2" s="13" t="n">
-        <v>46302</v>
-      </c>
-      <c r="D2" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="15" t="str">
-        <f aca="false">IF(G2="","",(G2/B2))</f>
-        <v/>
-      </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="XEJ2" s="0"/>
-      <c r="XEK2" s="0"/>
-      <c r="XEL2" s="0"/>
-      <c r="XEM2" s="0"/>
-      <c r="XEN2" s="0"/>
-      <c r="XEO2" s="0"/>
-      <c r="XEP2" s="0"/>
-      <c r="XEQ2" s="0"/>
-      <c r="XER2" s="0"/>
-      <c r="XES2" s="0"/>
-      <c r="XET2" s="0"/>
-      <c r="XEU2" s="0"/>
-      <c r="XEV2" s="0"/>
-      <c r="XEW2" s="0"/>
-      <c r="XEX2" s="0"/>
-      <c r="XEY2" s="0"/>
-      <c r="XEZ2" s="0"/>
-      <c r="XFA2" s="0"/>
-      <c r="XFB2" s="0"/>
-      <c r="XFC2" s="0"/>
-      <c r="XFD2" s="0"/>
-    </row>
-    <row r="3" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="12" t="n">
-        <v>40313</v>
-      </c>
-      <c r="C3" s="13" t="n">
-        <v>58197</v>
-      </c>
-      <c r="D3" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="15" t="str">
-        <f aca="false">IF(G3="","",(G3/B3))</f>
-        <v/>
-      </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="XEJ3" s="0"/>
-      <c r="XEK3" s="0"/>
-      <c r="XEL3" s="0"/>
-      <c r="XEM3" s="0"/>
-      <c r="XEN3" s="0"/>
-      <c r="XEO3" s="0"/>
-      <c r="XEP3" s="0"/>
-      <c r="XEQ3" s="0"/>
-      <c r="XER3" s="0"/>
-      <c r="XES3" s="0"/>
-      <c r="XET3" s="0"/>
-      <c r="XEU3" s="0"/>
-      <c r="XEV3" s="0"/>
-      <c r="XEW3" s="0"/>
-      <c r="XEX3" s="0"/>
-      <c r="XEY3" s="0"/>
-      <c r="XEZ3" s="0"/>
-      <c r="XFA3" s="0"/>
-      <c r="XFB3" s="0"/>
-      <c r="XFC3" s="0"/>
-      <c r="XFD3" s="0"/>
-    </row>
-    <row r="4" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="12" t="n">
-        <v>35579</v>
-      </c>
-      <c r="C4" s="13" t="n">
-        <v>46790</v>
-      </c>
-      <c r="D4" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="15" t="str">
-        <f aca="false">IF(G4="","",(G4/B4))</f>
-        <v/>
-      </c>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="XEJ4" s="0"/>
-      <c r="XEK4" s="0"/>
-      <c r="XEL4" s="0"/>
-      <c r="XEM4" s="0"/>
-      <c r="XEN4" s="0"/>
-      <c r="XEO4" s="0"/>
-      <c r="XEP4" s="0"/>
-      <c r="XEQ4" s="0"/>
-      <c r="XER4" s="0"/>
-      <c r="XES4" s="0"/>
-      <c r="XET4" s="0"/>
-      <c r="XEU4" s="0"/>
-      <c r="XEV4" s="0"/>
-      <c r="XEW4" s="0"/>
-      <c r="XEX4" s="0"/>
-      <c r="XEY4" s="0"/>
-      <c r="XEZ4" s="0"/>
-      <c r="XFA4" s="0"/>
-      <c r="XFB4" s="0"/>
-      <c r="XFC4" s="0"/>
-      <c r="XFD4" s="0"/>
-    </row>
-    <row r="5" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="12" t="n">
-        <v>30808</v>
-      </c>
-      <c r="C5" s="13" t="n">
-        <v>46605</v>
-      </c>
-      <c r="D5" s="14" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="13" t="n">
-        <v>130471</v>
-      </c>
-      <c r="H5" s="15" t="n">
-        <f aca="false">IF(G5="","",(G5/B5))</f>
-        <v>4.23497143599065</v>
-      </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="XEJ5" s="0"/>
-      <c r="XEK5" s="0"/>
-      <c r="XEL5" s="0"/>
-      <c r="XEM5" s="0"/>
-      <c r="XEN5" s="0"/>
-      <c r="XEO5" s="0"/>
-      <c r="XEP5" s="0"/>
-      <c r="XEQ5" s="0"/>
-      <c r="XER5" s="0"/>
-      <c r="XES5" s="0"/>
-      <c r="XET5" s="0"/>
-      <c r="XEU5" s="0"/>
-      <c r="XEV5" s="0"/>
-      <c r="XEW5" s="0"/>
-      <c r="XEX5" s="0"/>
-      <c r="XEY5" s="0"/>
-      <c r="XEZ5" s="0"/>
-      <c r="XFA5" s="0"/>
-      <c r="XFB5" s="0"/>
-      <c r="XFC5" s="0"/>
-      <c r="XFD5" s="0"/>
-    </row>
-    <row r="6" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="12" t="n">
-        <v>25041</v>
-      </c>
-      <c r="C6" s="13" t="n">
-        <v>104971</v>
-      </c>
-      <c r="D6" s="14" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="13" t="n">
-        <v>130784</v>
-      </c>
-      <c r="H6" s="15" t="n">
-        <f aca="false">IF(G6="","",(G6/B6))</f>
-        <v>5.2227946168284</v>
-      </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="XEJ6" s="0"/>
-      <c r="XEK6" s="0"/>
-      <c r="XEL6" s="0"/>
-      <c r="XEM6" s="0"/>
-      <c r="XEN6" s="0"/>
-      <c r="XEO6" s="0"/>
-      <c r="XEP6" s="0"/>
-      <c r="XEQ6" s="0"/>
-      <c r="XER6" s="0"/>
-      <c r="XES6" s="0"/>
-      <c r="XET6" s="0"/>
-      <c r="XEU6" s="0"/>
-      <c r="XEV6" s="0"/>
-      <c r="XEW6" s="0"/>
-      <c r="XEX6" s="0"/>
-      <c r="XEY6" s="0"/>
-      <c r="XEZ6" s="0"/>
-      <c r="XFA6" s="0"/>
-      <c r="XFB6" s="0"/>
-      <c r="XFC6" s="0"/>
-      <c r="XFD6" s="0"/>
-    </row>
-    <row r="7" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="12" t="n">
-        <v>19011</v>
-      </c>
-      <c r="C7" s="13" t="n">
-        <v>96136</v>
-      </c>
-      <c r="D7" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="13" t="n">
-        <v>124692</v>
-      </c>
-      <c r="H7" s="15" t="n">
-        <f aca="false">IF(G7="","",(G7/B7))</f>
-        <v>6.55893956130661</v>
-      </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="XEJ7" s="0"/>
-      <c r="XEK7" s="0"/>
-      <c r="XEL7" s="0"/>
-      <c r="XEM7" s="0"/>
-      <c r="XEN7" s="0"/>
-      <c r="XEO7" s="0"/>
-      <c r="XEP7" s="0"/>
-      <c r="XEQ7" s="0"/>
-      <c r="XER7" s="0"/>
-      <c r="XES7" s="0"/>
-      <c r="XET7" s="0"/>
-      <c r="XEU7" s="0"/>
-      <c r="XEV7" s="0"/>
-      <c r="XEW7" s="0"/>
-      <c r="XEX7" s="0"/>
-      <c r="XEY7" s="0"/>
-      <c r="XEZ7" s="0"/>
-      <c r="XFA7" s="0"/>
-      <c r="XFB7" s="0"/>
-      <c r="XFC7" s="0"/>
-      <c r="XFD7" s="0"/>
-    </row>
-    <row r="8" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="12" t="n">
-        <v>17953</v>
-      </c>
-      <c r="C8" s="13" t="n">
-        <v>54172</v>
-      </c>
-      <c r="D8" s="14" t="n">
-        <v>7</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="13" t="n">
-        <v>79451</v>
-      </c>
-      <c r="H8" s="15" t="n">
-        <f aca="false">IF(G8="","",(G8/B8))</f>
-        <v>4.4254999164485</v>
-      </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="XEJ8" s="0"/>
-      <c r="XEK8" s="0"/>
-      <c r="XEL8" s="0"/>
-      <c r="XEM8" s="0"/>
-      <c r="XEN8" s="0"/>
-      <c r="XEO8" s="0"/>
-      <c r="XEP8" s="0"/>
-      <c r="XEQ8" s="0"/>
-      <c r="XER8" s="0"/>
-      <c r="XES8" s="0"/>
-      <c r="XET8" s="0"/>
-      <c r="XEU8" s="0"/>
-      <c r="XEV8" s="0"/>
-      <c r="XEW8" s="0"/>
-      <c r="XEX8" s="0"/>
-      <c r="XEY8" s="0"/>
-      <c r="XEZ8" s="0"/>
-      <c r="XFA8" s="0"/>
-      <c r="XFB8" s="0"/>
-      <c r="XFC8" s="0"/>
-      <c r="XFD8" s="0"/>
-    </row>
-    <row r="9" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="12" t="n">
-        <v>17066</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>61386</v>
-      </c>
-      <c r="D9" s="14" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="13" t="n">
-        <v>107668</v>
-      </c>
-      <c r="H9" s="15" t="n">
-        <f aca="false">IF(G9="","",(G9/B9))</f>
-        <v>6.30891831712176</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="XEJ9" s="0"/>
-      <c r="XEK9" s="0"/>
-      <c r="XEL9" s="0"/>
-      <c r="XEM9" s="0"/>
-      <c r="XEN9" s="0"/>
-      <c r="XEO9" s="0"/>
-      <c r="XEP9" s="0"/>
-      <c r="XEQ9" s="0"/>
-      <c r="XER9" s="0"/>
-      <c r="XES9" s="0"/>
-      <c r="XET9" s="0"/>
-      <c r="XEU9" s="0"/>
-      <c r="XEV9" s="0"/>
-      <c r="XEW9" s="0"/>
-      <c r="XEX9" s="0"/>
-      <c r="XEY9" s="0"/>
-      <c r="XEZ9" s="0"/>
-      <c r="XFA9" s="0"/>
-      <c r="XFB9" s="0"/>
-      <c r="XFC9" s="0"/>
-      <c r="XFD9" s="0"/>
-    </row>
-    <row r="10" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="12" t="n">
-        <v>15930</v>
-      </c>
-      <c r="C10" s="13" t="n">
-        <v>49576</v>
-      </c>
-      <c r="D10" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="13" t="n">
-        <v>115294</v>
-      </c>
-      <c r="H10" s="15" t="n">
-        <f aca="false">IF(G10="","",(G10/B10))</f>
-        <v>7.2375392341494</v>
-      </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="XEJ10" s="0"/>
-      <c r="XEK10" s="0"/>
-      <c r="XEL10" s="0"/>
-      <c r="XEM10" s="0"/>
-      <c r="XEN10" s="0"/>
-      <c r="XEO10" s="0"/>
-      <c r="XEP10" s="0"/>
-      <c r="XEQ10" s="0"/>
-      <c r="XER10" s="0"/>
-      <c r="XES10" s="0"/>
-      <c r="XET10" s="0"/>
-      <c r="XEU10" s="0"/>
-      <c r="XEV10" s="0"/>
-      <c r="XEW10" s="0"/>
-      <c r="XEX10" s="0"/>
-      <c r="XEY10" s="0"/>
-      <c r="XEZ10" s="0"/>
-      <c r="XFA10" s="0"/>
-      <c r="XFB10" s="0"/>
-      <c r="XFC10" s="0"/>
-      <c r="XFD10" s="0"/>
-    </row>
-    <row r="11" s="20" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="12" t="n">
-        <v>13896</v>
-      </c>
-      <c r="C11" s="13" t="n">
-        <v>82189</v>
-      </c>
-      <c r="D11" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="13" t="n">
-        <v>192268</v>
-      </c>
-      <c r="H11" s="15" t="n">
-        <f aca="false">IF(G11="","",(G11/B11))</f>
-        <v>13.8362118595279</v>
-      </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="XEJ11" s="0"/>
-      <c r="XEK11" s="0"/>
-      <c r="XEL11" s="0"/>
-      <c r="XEM11" s="0"/>
-      <c r="XEN11" s="0"/>
-      <c r="XEO11" s="0"/>
-      <c r="XEP11" s="0"/>
-      <c r="XEQ11" s="0"/>
-      <c r="XER11" s="0"/>
-      <c r="XES11" s="0"/>
-      <c r="XET11" s="0"/>
-      <c r="XEU11" s="0"/>
-      <c r="XEV11" s="0"/>
-      <c r="XEW11" s="0"/>
-      <c r="XEX11" s="0"/>
-      <c r="XEY11" s="0"/>
-      <c r="XEZ11" s="0"/>
-      <c r="XFA11" s="0"/>
-      <c r="XFB11" s="0"/>
-      <c r="XFC11" s="0"/>
-      <c r="XFD11" s="0"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E2:E11">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K11">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L11">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M11">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O11">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P11">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S11">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T11">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U11">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF00A933"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>